<commit_message>
[IMP] Adjust cheque register report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cheque_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cheque_register.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">รายงานทะเบียนคุมเช็ค</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Cheque Register Report</t>
   </si>
   <si>
     <t xml:space="preserve">Cheque Received Date</t>
@@ -80,8 +80,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -167,15 +169,31 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,7 +202,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -213,7 +235,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -225,100 +247,106 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="4" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="10" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] #2601 Change filter
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_cheque_register.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_cheque_register.xlsx
@@ -20,51 +20,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">Cheque Register Report</t>
   </si>
   <si>
+    <t xml:space="preserve">Cheque Received Date From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheque Received Date To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheque Number From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheque Number To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheque Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Payment Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posting Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheque Amount</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cheque Received Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lot Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheque Number From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheque Number To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run By</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheque Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier Payment Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posting Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheque Amount</t>
   </si>
   <si>
     <t xml:space="preserve">Encashed Date</t>
@@ -238,12 +244,12 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.79"/>
@@ -272,81 +278,85 @@
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>